<commit_message>
Week 2 day 1
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/19bf9171b6e18731/Documenten/Masterproef/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenni\OneDrive\Documenten\Masterproef\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="AECADA6CA3C902291FFEFFA2CD533AC8B958C4B4" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{B30B70C7-5D29-4AD0-BBAE-C7CA47AE9C92}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="AECADA6CA3C902291FFEFFA2CD533AC8B958C4B4" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{49CB4927-A4CD-4110-9E91-183157AC269A}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7905" xr2:uid="{FCF6F198-3308-44C1-B7C4-8A97FA86A381}"/>
   </bookViews>
@@ -90,9 +90,6 @@
     <t>Implementatie Xamarin</t>
   </si>
   <si>
-    <t>Implementatie PhoneGap</t>
-  </si>
-  <si>
     <t>Implementatie Qt</t>
   </si>
   <si>
@@ -106,13 +103,16 @@
   </si>
   <si>
     <t>Wetenschappelijke tekst schrijven</t>
+  </si>
+  <si>
+    <t>Implementatie Apache Cordova</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,16 +128,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -160,24 +196,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Goed" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutraal" xfId="3" builtinId="28"/>
+    <cellStyle name="Ongeldig" xfId="2" builtinId="27"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -493,7 +554,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +563,7 @@
     <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.7109375" customWidth="1"/>
     <col min="4" max="4" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32.140625" bestFit="1" customWidth="1"/>
@@ -532,17 +593,17 @@
         <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I1" s="3">
         <v>42878</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -561,15 +622,15 @@
         <v>17</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -577,22 +638,22 @@
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="4"/>
@@ -601,13 +662,13 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="4"/>
@@ -619,8 +680,8 @@
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="4"/>

</xml_diff>